<commit_message>
OwnerDepositYieldComputer major bug fix
</commit_message>
<xml_diff>
--- a/test/testdata/testSBEarningUsdc_uniqueOwner_2_deposit.xlsx
+++ b/test/testdata/testSBEarningUsdc_uniqueOwner_2_deposit.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Transactions" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Transactions!$A$1:$V$66</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -327,14 +330,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="#0.##"/>
     <numFmt numFmtId="165" formatCode="#0.#######"/>
     <numFmt numFmtId="166" formatCode="#0.###"/>
     <numFmt numFmtId="167" formatCode="#0.########"/>
-    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="168" formatCode="yyyy\-mm\-\d\d\ hh:mm:ss"/>
+    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="170" formatCode="0.00000000000000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -399,6 +404,14 @@
       <name val="Calibri"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -445,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -471,12 +484,17 @@
     <xf numFmtId="167" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="168" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="169" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -797,16 +815,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D30" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B34" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="2" width="29.07421875" customWidth="1"/>
-    <col min="3" max="10" width="14.921875" customWidth="1"/>
+    <col min="3" max="8" width="14.921875" customWidth="1"/>
+    <col min="9" max="9" width="18.15234375" customWidth="1"/>
+    <col min="10" max="10" width="17.4609375" customWidth="1"/>
     <col min="11" max="11" width="69.921875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -851,19 +871,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="9" spans="1:11" ht="26.15" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
@@ -2041,8 +2061,8 @@
       <c r="H42" s="5">
         <v>0</v>
       </c>
-      <c r="I42" s="5">
-        <v>8.4393401451999992</v>
+      <c r="I42" s="11">
+        <v>10.9807680876656</v>
       </c>
       <c r="J42" s="5"/>
       <c r="K42" s="4" t="s">
@@ -2070,8 +2090,8 @@
       <c r="H43" s="5">
         <v>0</v>
       </c>
-      <c r="I43">
-        <v>13.003941849</v>
+      <c r="I43" s="11">
+        <v>14.9665097292781</v>
       </c>
       <c r="J43" s="5"/>
       <c r="K43" s="4" t="s">
@@ -2099,8 +2119,8 @@
       <c r="H44" s="5">
         <v>0</v>
       </c>
-      <c r="I44" s="5">
-        <v>10.869080305800001</v>
+      <c r="I44" s="11">
+        <v>12.647539121578999</v>
       </c>
       <c r="J44" s="5"/>
       <c r="K44" s="4" t="s">
@@ -2128,8 +2148,8 @@
       <c r="H45" s="5">
         <v>0</v>
       </c>
-      <c r="I45" s="5">
-        <v>14.0996818583</v>
+      <c r="I45" s="11">
+        <v>9.8349663136505097</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="4" t="s">
@@ -2157,12 +2177,22 @@
       <c r="H46" s="5">
         <v>0</v>
       </c>
-      <c r="I46" s="5">
-        <v>10.382022056</v>
+      <c r="I46" s="11">
+        <v>14.994624157308801</v>
       </c>
       <c r="J46" s="5"/>
       <c r="K46" s="4" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="I47" s="12">
+        <f>SUM(I42:I46)</f>
+        <v>63.424407409482008</v>
+      </c>
+      <c r="J47" s="13">
+        <f>SUM(I42:I46)</f>
+        <v>63.424407409482008</v>
       </c>
     </row>
   </sheetData>
@@ -2171,6 +2201,6 @@
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="22" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>